<commit_message>
Atualização das regras de negócio, CSU e Diagrama de classe
</commit_message>
<xml_diff>
--- a/Documentation/Regra de Negócios 1.2.xlsx
+++ b/Documentation/Regra de Negócios 1.2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artur\Documents\Projeto\e-star\Documentation\Contributors\ARTUR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UNP\6º SEMESTRE\ENG DE SOFTWARE\DOCUMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -33,9 +33,6 @@
     <t>RN[1.2]. Cadastrar TCC</t>
   </si>
   <si>
-    <t>Um TCC deve ser cadastrado com os campos de acordo com o anexo I do Edital de abertura do TCC. Obrigatório preenchimento de todos os campos, com exceção de um dos alunos. O aluno deve cadastrar e o professor validar. Em caso de negação, justificar. A efetivação do cadastro se dará pela coordenação.</t>
-  </si>
-  <si>
     <t>RN[1.3]. Termos e condições</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>RN[1.4]. Submissão de trabalhos</t>
   </si>
   <si>
-    <t>Todos os trabalhos devem ser submetidos no sistema na forma de PDF. A cada nova submissão um email deve ser disparado para o orientador e a equipe pedagógica.</t>
-  </si>
-  <si>
     <t>RN[1.5]. Marcação de intervenções</t>
   </si>
   <si>
@@ -132,14 +126,20 @@
     <t>RN[1.1.1]. Realizar login</t>
   </si>
   <si>
-    <t>O usuário</t>
+    <t>O usuário deve logar com seu login e senha para acessar o sistema.</t>
+  </si>
+  <si>
+    <t>Um TCC deve ser cadastrado com os campos de acordo com o anexo I (LINHA DE PESQUISA POR CURSO,II (FORMULÁRIO DE PROPOSTA DE TRABALHO, III (TERMO DE COMPROMISSO DE ORIENTAÇÃO), do Edital de abertura do TCC. Obrigatório preenchimento de todos os campos, com exceção de um dos alunos. O aluno deve cadastrar e o professor validar. Em caso de negação, justificar. A efetivação do cadastro se dará pela coordenação.</t>
+  </si>
+  <si>
+    <t>Todos os trabalhos devem ser submetidos no sistema na forma de PDF e resolução maxima permitida, indicando sua revisão. A cada nova submissão um email deve ser disparado para o orientador e a equipe pedagógica informando avanço de revisão.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -157,6 +157,24 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -337,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -349,11 +367,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -362,19 +389,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -659,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -673,76 +708,76 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="12"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
+      <c r="B3" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="12"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
-      <c r="B4" s="21"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="9"/>
+      <c r="B5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="12"/>
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
+      <c r="B6" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="12"/>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -752,46 +787,46 @@
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="12"/>
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="12"/>
+      <c r="A9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="15"/>
+    <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -804,30 +839,30 @@
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="9"/>
+      <c r="B12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="12"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="9"/>
+      <c r="B13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="12"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -837,30 +872,30 @@
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="9"/>
+      <c r="B15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="12"/>
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="9"/>
+      <c r="B16" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="12"/>
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -870,65 +905,65 @@
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
+      <c r="B18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="12"/>
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9"/>
+      <c r="B19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="12"/>
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="2"/>
+    <row r="21" spans="1:14" s="27" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="N21" s="28"/>
+    </row>
+    <row r="22" spans="1:14" s="27" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="28"/>
     </row>
     <row r="23" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="N23" s="2"/>
@@ -937,47 +972,47 @@
       <c r="A24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
+      <c r="B24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="12"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="12"/>
+      <c r="A25" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="17"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="15"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="20"/>
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -990,30 +1025,30 @@
       <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="9"/>
+      <c r="B28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="12"/>
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="9"/>
+      <c r="B29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="12"/>
       <c r="N29" s="2"/>
     </row>
     <row r="30" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1023,30 +1058,30 @@
       <c r="A31" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="9"/>
+      <c r="B31" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="12"/>
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="9"/>
+      <c r="B32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="12"/>
       <c r="N32" s="2"/>
     </row>
     <row r="33" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1056,47 +1091,47 @@
       <c r="A34" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
+      <c r="B34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="12"/>
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="12"/>
+      <c r="A35" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="17"/>
       <c r="N35" s="2"/>
     </row>
     <row r="36" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="15"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="20"/>
       <c r="N36" s="2"/>
     </row>
     <row r="37" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1109,30 +1144,30 @@
       <c r="A38" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="9"/>
+      <c r="B38" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="12"/>
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="9"/>
+      <c r="B39" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="12"/>
       <c r="N39" s="2"/>
     </row>
     <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1142,30 +1177,30 @@
       <c r="A41" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="9"/>
+      <c r="B41" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="12"/>
       <c r="N41" s="2"/>
     </row>
     <row r="42" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="9"/>
+      <c r="B42" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="12"/>
       <c r="N42" s="2"/>
     </row>
     <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1175,30 +1210,30 @@
       <c r="A44" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="9"/>
+      <c r="B44" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="12"/>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="9"/>
+      <c r="B45" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="12"/>
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1208,31 +1243,31 @@
       <c r="A47" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
+      <c r="B47" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="12"/>
       <c r="N47" s="2"/>
     </row>
     <row r="48" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="9"/>
+      <c r="B48" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="12"/>
       <c r="N48" s="2"/>
     </row>
     <row r="49" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1242,31 +1277,31 @@
       <c r="A50" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
+      <c r="B50" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="12"/>
       <c r="N50" s="2"/>
     </row>
     <row r="51" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="9"/>
+      <c r="B51" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="12"/>
       <c r="N51" s="2"/>
     </row>
     <row r="52" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1276,30 +1311,30 @@
       <c r="A53" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53" s="9"/>
+      <c r="B53" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="12"/>
       <c r="N53" s="2"/>
     </row>
     <row r="54" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="9"/>
+      <c r="B54" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="12"/>
       <c r="N54" s="2"/>
     </row>
     <row r="55" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1309,30 +1344,30 @@
       <c r="A56" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C56" s="9"/>
+      <c r="B56" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="12"/>
       <c r="N56" s="2"/>
     </row>
     <row r="57" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="9"/>
+      <c r="B57" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="12"/>
       <c r="N57" s="2"/>
     </row>
   </sheetData>
@@ -1367,16 +1402,17 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B50:D50"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B45:M45"/>
     <mergeCell ref="B48:M48"/>
     <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B50:D50"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B35:M36"/>
     <mergeCell ref="B39:M39"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>